<commit_message>
read Cell By column name and row number function added
</commit_message>
<xml_diff>
--- a/Excel/DATA_TEST.xlsx
+++ b/Excel/DATA_TEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AutomationTasks\Nopecommerce\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF499BE-79D4-46E6-B76B-DC77D5DB0D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BF22AA-1023-4746-B9AD-08FA3197DBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4965" yWindow="2730" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,22 +28,22 @@
     <t>mail</t>
   </si>
   <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
     <t>test3@gmail.clom</t>
   </si>
   <si>
     <t>test2@gmail.com</t>
   </si>
   <si>
-    <t>test123</t>
-  </si>
-  <si>
     <t>test234</t>
   </si>
   <si>
     <t>test345</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>ahmedmohamed363@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:H422"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -428,10 +428,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -442,10 +442,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -456,10 +456,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>

</xml_diff>